<commit_message>
Commit data, update entity, service, repository
</commit_message>
<xml_diff>
--- a/Pokemon_Server/data/pkm_ability_changelog.xlsx
+++ b/Pokemon_Server/data/pkm_ability_changelog.xlsx
@@ -70,12 +70,6 @@
     <t>Has no effect in battle.</t>
   </si>
   <si>
-    <t>Doubles []{move:cut}'s grass-cutting radius on the overworld if any party Pokémon has this ability.</t>
-  </si>
-  <si>
-    <t>Does not affect friendly Pokémon's moves that target all other Pokémon.  This ability's presence is not announced upon entering battle.</t>
-  </si>
-  <si>
     <t>Prevents []{move:heal-bell} from curing the Pokémon, whether or not it is in battle.</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>[]{move:fire-fang} and moves that inflict [typeless damage]{mechanic:typeless-damage} ignore this ability regardless of type.</t>
   </si>
   <si>
-    <t>Inflicts only 1/16 of the attacker's maximum [HP]{mechanic:hp} in damage.</t>
-  </si>
-  <si>
     <t>Affects other Pokémon with this ability.</t>
   </si>
   <si>
@@ -125,6 +116,15 @@
   </si>
   <si>
     <t>ability_changelog_id</t>
+  </si>
+  <si>
+    <t>Inflicts only 1/16 of the attacker''s maximum [HP]{mechanic:hp} in damage.</t>
+  </si>
+  <si>
+    <t>Does not affect friendly Pokémon''s moves that target all other Pokémon.  This ability''s presence is not announced upon entering battle.</t>
+  </si>
+  <si>
+    <t>Doubles []{move:cut}''s grass-cutting radius on the overworld if any party Pokémon has this ability.</t>
   </si>
 </sst>
 </file>
@@ -486,16 +486,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -551,7 +551,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,7 +691,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>